<commit_message>
api for credit card repayment
</commit_message>
<xml_diff>
--- a/api/credit-card/credit-card.xlsx
+++ b/api/credit-card/credit-card.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>Who</t>
   </si>
@@ -98,9 +98,6 @@
     <t>user wants to view specific transactions of specific card</t>
   </si>
   <si>
-    <t>/users/{uid}/cards/{cid}/repayment</t>
-  </si>
-  <si>
     <t>user wants to repay to a card</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>user wants to view a repay to a card</t>
   </si>
   <si>
-    <t>/users/{uid}/cards/{cid}/repayment/{rid}</t>
-  </si>
-  <si>
     <t>create a statement of a card for a user</t>
   </si>
   <si>
@@ -167,12 +161,6 @@
     <t>/users/{uid}/cards/{cid}/instalment-contracts</t>
   </si>
   <si>
-    <t>view instalment contract of a statement</t>
-  </si>
-  <si>
-    <t>view instalment contracts of a statement</t>
-  </si>
-  <si>
     <t>/users/{uid}/cards/{cid}/instalment-contracts/{icid}/instalments/{iid}</t>
   </si>
   <si>
@@ -186,6 +174,21 @@
   </si>
   <si>
     <t>view instalment of instalment contract</t>
+  </si>
+  <si>
+    <t>/users/{uid}/cards/{cid}/repayments</t>
+  </si>
+  <si>
+    <t>/users/{uid}/cards/{cid}/repayments/{rid}</t>
+  </si>
+  <si>
+    <t>user wants to view repayments</t>
+  </si>
+  <si>
+    <t>view instalment contracts</t>
+  </si>
+  <si>
+    <t>view instalment contract</t>
   </si>
 </sst>
 </file>
@@ -532,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="112" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,13 +716,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2">
         <v>201400404</v>
@@ -730,53 +733,53 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2">
         <v>200404</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="2"/>
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2">
+        <v>200404</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="2">
-        <v>201400404</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2">
-        <v>200404</v>
+        <v>201400404</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -784,13 +787,13 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2">
         <v>200404</v>
@@ -801,13 +804,13 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="2">
         <v>200404</v>
@@ -818,13 +821,13 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2">
         <v>200404</v>
@@ -835,13 +838,13 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2">
         <v>200404</v>
@@ -852,13 +855,13 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2">
         <v>200404</v>
@@ -869,16 +872,16 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2">
-        <v>201400404</v>
+        <v>200404</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -886,16 +889,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2">
-        <v>200404</v>
+        <v>201400404</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -903,16 +906,16 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E24" s="2">
-        <v>201400404</v>
+        <v>200404</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -920,16 +923,16 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E25" s="2">
-        <v>200404</v>
+        <v>201400404</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -937,13 +940,13 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E26" s="2">
         <v>200404</v>
@@ -954,13 +957,13 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E27" s="2">
         <v>200404</v>
@@ -971,20 +974,34 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="2">
+        <v>200404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
         <v>49</v>
       </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="2">
-        <v>200404</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>200404</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="2"/>
@@ -1021,6 +1038,9 @@
     </row>
     <row r="41" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>